<commit_message>
Make filter table for data-pendaftar page
</commit_message>
<xml_diff>
--- a/exports/xlsx/data_pendaftar_ktmse.xlsx
+++ b/exports/xlsx/data_pendaftar_ktmse.xlsx
@@ -7,10 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Pribadi" sheetId="1" r:id="rId4"/>
-    <sheet name="Data Sekolah" sheetId="2" r:id="rId5"/>
-    <sheet name="Program Studi" sheetId="3" r:id="rId6"/>
-    <sheet name="Data Prestasi" sheetId="4" r:id="rId7"/>
+    <sheet name="Data Pendaftar" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -18,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>No.</t>
   </si>
@@ -126,6 +123,135 @@
   </si>
   <si>
     <t>Prestasi 5</t>
+  </si>
+  <si>
+    <t>Surat Keterangan Miskin</t>
+  </si>
+  <si>
+    <t>Surat Keterangan Penghasilan Keluarga</t>
+  </si>
+  <si>
+    <t>Foto Rumah</t>
+  </si>
+  <si>
+    <t>Data KTMSE 1</t>
+  </si>
+  <si>
+    <t>Jln Anggur Perumahan Semesta Blok A11, Palembang, Sumatera Selatan</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>0111111111111</t>
+  </si>
+  <si>
+    <t>Wanita</t>
+  </si>
+  <si>
+    <t>Lubuk Linggau</t>
+  </si>
+  <si>
+    <t>2001-11-11</t>
+  </si>
+  <si>
+    <t>pas_foto_007.jpg</t>
+  </si>
+  <si>
+    <t>KTMSE</t>
+  </si>
+  <si>
+    <t>Sekolah Menengah Kejuruan (SMK)</t>
+  </si>
+  <si>
+    <t>SMK Farmasi</t>
+  </si>
+  <si>
+    <t>SMAN 1 Palembang</t>
+  </si>
+  <si>
+    <t>Negeri</t>
+  </si>
+  <si>
+    <t>Sumatera Selatan</t>
+  </si>
+  <si>
+    <t>Kota Palembang</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>rekap_nilai_rapot_007.xlsx</t>
+  </si>
+  <si>
+    <t>bukti_pembayaran_007.jpg</t>
+  </si>
+  <si>
+    <t>Prodi DIII Farmasi</t>
+  </si>
+  <si>
+    <t>surat_keterangan_miskin_007.pdf</t>
+  </si>
+  <si>
+    <t>surat_keterangan_penghasilan_keluarga_007.pdf</t>
+  </si>
+  <si>
+    <t>foto_rumah_007.pdf</t>
+  </si>
+  <si>
+    <t>Data KTMSE 2</t>
+  </si>
+  <si>
+    <t>Jln Apel Gg Kosong Rumah Nomor 12, Banyuasin, Sumatera Selatan</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>022222222222</t>
+  </si>
+  <si>
+    <t>Pagar Alam</t>
+  </si>
+  <si>
+    <t>2001-07-03</t>
+  </si>
+  <si>
+    <t>pas_foto_008.jpg</t>
+  </si>
+  <si>
+    <t>Madrasah Aliyah Kejuruan (MAK)</t>
+  </si>
+  <si>
+    <t>SMK Keperawatan Gigi</t>
+  </si>
+  <si>
+    <t>SMAN 3 Palembang</t>
+  </si>
+  <si>
+    <t>rekap_nilai_rapot_008.xlsx</t>
+  </si>
+  <si>
+    <t>bukti_pembayaran_008.jpg</t>
+  </si>
+  <si>
+    <t>Prodi DIII Keperawatan Palembang</t>
+  </si>
+  <si>
+    <t>prestasi_1_008.pdf</t>
+  </si>
+  <si>
+    <t>prestasi_2_008.pdf</t>
+  </si>
+  <si>
+    <t>surat_keterangan_miskin_008.pdf</t>
+  </si>
+  <si>
+    <t>surat_keterangan_penghasilan_keluarga_008.pdf</t>
+  </si>
+  <si>
+    <t>foto_rumah_008.pdf</t>
   </si>
 </sst>
 </file>
@@ -464,7 +590,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +598,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:39">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,185 +638,301 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
     </row>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
+    <row r="2" spans="1:39">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>11111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>165</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2">
+        <v>2019</v>
+      </c>
+      <c r="V2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W2">
+        <v>96.5</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>60</v>
       </c>
     </row>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
+    <row r="3" spans="1:39">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3">
+        <v>11112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>160</v>
+      </c>
+      <c r="I3">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3">
+        <v>2019</v>
+      </c>
+      <c r="V3" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3">
+        <v>94.5</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE3"/>
+      <c r="AF3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beautify url using segment
</commit_message>
<xml_diff>
--- a/exports/xlsx/data_pendaftar_ktmse.xlsx
+++ b/exports/xlsx/data_pendaftar_ktmse.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>No.</t>
   </si>
@@ -132,126 +132,6 @@
   </si>
   <si>
     <t>Foto Rumah</t>
-  </si>
-  <si>
-    <t>Data KTMSE 1</t>
-  </si>
-  <si>
-    <t>Jln Anggur Perumahan Semesta Blok A11, Palembang, Sumatera Selatan</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>0111111111111</t>
-  </si>
-  <si>
-    <t>Wanita</t>
-  </si>
-  <si>
-    <t>Lubuk Linggau</t>
-  </si>
-  <si>
-    <t>2001-11-11</t>
-  </si>
-  <si>
-    <t>pas_foto_007.jpg</t>
-  </si>
-  <si>
-    <t>KTMSE</t>
-  </si>
-  <si>
-    <t>Sekolah Menengah Kejuruan (SMK)</t>
-  </si>
-  <si>
-    <t>SMK Farmasi</t>
-  </si>
-  <si>
-    <t>SMAN 1 Palembang</t>
-  </si>
-  <si>
-    <t>Negeri</t>
-  </si>
-  <si>
-    <t>Sumatera Selatan</t>
-  </si>
-  <si>
-    <t>Kota Palembang</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>rekap_nilai_rapot_007.xlsx</t>
-  </si>
-  <si>
-    <t>bukti_pembayaran_007.jpg</t>
-  </si>
-  <si>
-    <t>Prodi DIII Farmasi</t>
-  </si>
-  <si>
-    <t>surat_keterangan_miskin_007.pdf</t>
-  </si>
-  <si>
-    <t>surat_keterangan_penghasilan_keluarga_007.pdf</t>
-  </si>
-  <si>
-    <t>foto_rumah_007.pdf</t>
-  </si>
-  <si>
-    <t>Data KTMSE 2</t>
-  </si>
-  <si>
-    <t>Jln Apel Gg Kosong Rumah Nomor 12, Banyuasin, Sumatera Selatan</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>022222222222</t>
-  </si>
-  <si>
-    <t>Pagar Alam</t>
-  </si>
-  <si>
-    <t>2001-07-03</t>
-  </si>
-  <si>
-    <t>pas_foto_008.jpg</t>
-  </si>
-  <si>
-    <t>Madrasah Aliyah Kejuruan (MAK)</t>
-  </si>
-  <si>
-    <t>SMK Keperawatan Gigi</t>
-  </si>
-  <si>
-    <t>SMAN 3 Palembang</t>
-  </si>
-  <si>
-    <t>rekap_nilai_rapot_008.xlsx</t>
-  </si>
-  <si>
-    <t>bukti_pembayaran_008.jpg</t>
-  </si>
-  <si>
-    <t>Prodi DIII Keperawatan Palembang</t>
-  </si>
-  <si>
-    <t>prestasi_1_008.pdf</t>
-  </si>
-  <si>
-    <t>prestasi_2_008.pdf</t>
-  </si>
-  <si>
-    <t>surat_keterangan_miskin_008.pdf</t>
-  </si>
-  <si>
-    <t>surat_keterangan_penghasilan_keluarga_008.pdf</t>
-  </si>
-  <si>
-    <t>foto_rumah_008.pdf</t>
   </si>
 </sst>
 </file>
@@ -590,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,224 +595,6 @@
       </c>
       <c r="AM1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>11111</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2">
-        <v>165</v>
-      </c>
-      <c r="I2">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2">
-        <v>2019</v>
-      </c>
-      <c r="V2" t="s">
-        <v>55</v>
-      </c>
-      <c r="W2">
-        <v>96.5</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3">
-        <v>11112</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3">
-        <v>160</v>
-      </c>
-      <c r="I3">
-        <v>40</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O3" t="s">
-        <v>69</v>
-      </c>
-      <c r="P3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T3" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3">
-        <v>2019</v>
-      </c>
-      <c r="V3" t="s">
-        <v>71</v>
-      </c>
-      <c r="W3">
-        <v>94.5</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>1</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE3"/>
-      <c r="AF3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>